<commit_message>
Added the input TVS-diode. Regenerated BOM and SCH files.
</commit_message>
<xml_diff>
--- a/OUTPUT/BOM/Gastroscopy-Controller_BOM_Rev_0.1.0_No Variations.xlsx
+++ b/OUTPUT/BOM/Gastroscopy-Controller_BOM_Rev_0.1.0_No Variations.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">11.11.2022</t>
   </si>
   <si>
-    <t xml:space="preserve">7:11</t>
+    <t xml:space="preserve">12:59</t>
   </si>
   <si>
     <t xml:space="preserve">Print Date:</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">CC0603JRNPO9BN300</t>
   </si>
   <si>
-    <t xml:space="preserve">D1, D2, D3, D4, D5, D6, D14</t>
+    <t xml:space="preserve">D1, D2, D3, D4, D5, D6, D14, D15</t>
   </si>
   <si>
     <t xml:space="preserve">TVS DIODE 5VWM 9.2VC SMB</t>
@@ -515,7 +515,7 @@
     <t xml:space="preserve">Total Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">141</t>
+    <t xml:space="preserve">142</t>
   </si>
   <si>
     <t xml:space="preserve">Report Time</t>
@@ -527,7 +527,7 @@
     <t xml:space="preserve">Report Date &amp; Tine</t>
   </si>
   <si>
-    <t xml:space="preserve">11.11.2022 7:11</t>
+    <t xml:space="preserve">11.11.2022 12:59</t>
   </si>
   <si>
     <t xml:space="preserve">Output Name</t>
@@ -1103,8 +1103,8 @@
       <xdr:rowOff>77400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1101600</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>185040</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
@@ -1119,7 +1119,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6657840" y="77400"/>
+          <a:off x="6562800" y="77400"/>
           <a:ext cx="1915920" cy="1736640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1142,7 +1142,7 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="false" view="normal" topLeftCell="A28" colorId="8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="false" view="normal" topLeftCell="A22" colorId="8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1152,9 +1152,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="32.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="34.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="13.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="16.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7"/>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="E8" s="26" t="n">
         <f aca="true">NOW()</f>
-        <v>44876.3004779051</v>
+        <v>44876.5415613542</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="22"/>
@@ -1302,7 +1302,7 @@
       <c r="W9" s="29"/>
       <c r="X9" s="29"/>
     </row>
-    <row r="10" customFormat="false" ht="21.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="30" t="n">
         <f aca="false">ROW(B10) - ROW($B$9)</f>
@@ -1393,7 +1393,7 @@
         <v>33</v>
       </c>
       <c r="G13" s="35" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q13" s="29"/>
       <c r="X13" s="29"/>
@@ -1566,7 +1566,7 @@
       <c r="Q20" s="29"/>
       <c r="X20" s="29"/>
     </row>
-    <row r="21" customFormat="false" ht="31.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="32.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="33" t="n">
         <f aca="false">ROW(B21) - ROW($B$9)</f>
@@ -2225,7 +2225,7 @@
       <c r="F48" s="39"/>
       <c r="G48" s="40" t="n">
         <f aca="false">SUM(G10:G47)</f>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q48" s="29"/>
       <c r="W48" s="1"/>

</xml_diff>

<commit_message>
Сhanged the Main MCU.
</commit_message>
<xml_diff>
--- a/OUTPUT/BOM/Gastroscopy-Controller_BOM_Rev_0.1.0_No Variations.xlsx
+++ b/OUTPUT/BOM/Gastroscopy-Controller_BOM_Rev_0.1.0_No Variations.xlsx
@@ -446,10 +446,10 @@
     <t xml:space="preserve">U3</t>
   </si>
   <si>
-    <t xml:space="preserve">IC MCU 32BIT 32KB FLASH 48LQFP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F103C6T6A</t>
+    <t xml:space="preserve">IC MCU 32BIT 128KB FLASH 48LQFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F103CBT6</t>
   </si>
   <si>
     <t xml:space="preserve">U4</t>
@@ -1104,9 +1104,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>185040</xdr:colOff>
+      <xdr:colOff>184680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1119,8 +1119,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6562800" y="77400"/>
-          <a:ext cx="1915920" cy="1736640"/>
+          <a:off x="6563160" y="77400"/>
+          <a:ext cx="1915920" cy="1736280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1142,13 +1142,13 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="false" view="normal" topLeftCell="A22" colorId="8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="32.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="34.28"/>
@@ -1156,7 +1156,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.28"/>
@@ -1263,11 +1263,11 @@
       </c>
       <c r="D8" s="25" t="n">
         <f aca="true">TODAY()</f>
-        <v>44876</v>
+        <v>44881</v>
       </c>
       <c r="E8" s="26" t="n">
         <f aca="true">NOW()</f>
-        <v>44876.5415613542</v>
+        <v>44881.5959346528</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="22"/>
@@ -2260,7 +2260,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="false" view="normal" topLeftCell="A1" colorId="8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>